<commit_message>
Removendo coluna de distancia
Removendo coluna de distancia
</commit_message>
<xml_diff>
--- a/Pi.xlsx
+++ b/Pi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulo\OneDrive\Documentos\GitHub\Senac\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>Sol</t>
   </si>
@@ -75,53 +75,16 @@
   </si>
   <si>
     <t>Tamanho Latex</t>
-  </si>
-  <si>
-    <t>Distancia</t>
-  </si>
-  <si>
-    <t>149.6 </t>
-  </si>
-  <si>
-    <t>228.0 </t>
-  </si>
-  <si>
-    <t>778.4 </t>
-  </si>
-  <si>
-    <t>4496.6 </t>
-  </si>
-  <si>
-    <t>Distancia latex</t>
-  </si>
-  <si>
-    <t>57910 </t>
-  </si>
-  <si>
-    <t>1427.0 </t>
-  </si>
-  <si>
-    <t>2869.6 </t>
-  </si>
-  <si>
-    <t>10816 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -153,7 +116,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -189,36 +152,16 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,7 +445,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E13" sqref="E13:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,12 +730,6 @@
       <c r="D13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -805,11 +742,6 @@
       <c r="D14" s="4">
         <v>10</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="G14">
-        <f>1392000/2</f>
-        <v>696000</v>
-      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
@@ -826,12 +758,6 @@
         <f>C15*D$14</f>
         <v>3.5053160919540229E-2</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="8">
-        <v>12.018649628734201</v>
-      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -848,15 +774,8 @@
         <f t="shared" ref="D16:D22" si="2">C16*D$14</f>
         <v>8.6951149425287366E-2</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="9" t="e">
-        <f>G14/E16</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>3</v>
       </c>
@@ -871,11 +790,8 @@
         <f t="shared" si="2"/>
         <v>9.1639367816091971E-2</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>4</v>
       </c>
@@ -890,11 +806,8 @@
         <f t="shared" si="2"/>
         <v>4.8795977011494254E-2</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>5</v>
       </c>
@@ -909,11 +822,8 @@
         <f t="shared" si="2"/>
         <v>1.027183908045977</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
@@ -928,11 +838,8 @@
         <f t="shared" si="2"/>
         <v>0.86591954022988515</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>7</v>
       </c>
@@ -947,11 +854,8 @@
         <f t="shared" si="2"/>
         <v>0.36722701149425285</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>8</v>
       </c>
@@ -965,9 +869,6 @@
       <c r="D22" s="4">
         <f t="shared" si="2"/>
         <v>0.35580459770114947</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>